<commit_message>
02/06 Seguimiento de Cobro de Obligaciones y FrmEstadoDeCuenta Version4.9.833 2.5 h
</commit_message>
<xml_diff>
--- a/Version4.9.833/Precio IVA Tarjeta.xlsx
+++ b/Version4.9.833/Precio IVA Tarjeta.xlsx
@@ -372,6 +372,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -404,12 +410,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1155,7 +1155,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1172,20 +1172,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="47"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="49"/>
     </row>
     <row r="2" spans="1:15" ht="6.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1204,7 +1204,7 @@
       </c>
       <c r="J3" s="43"/>
       <c r="K3" s="44"/>
-      <c r="L3" s="56" t="s">
+      <c r="L3" s="45" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1215,17 +1215,17 @@
       <c r="B4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="49"/>
+      <c r="D4" s="51"/>
       <c r="E4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="48" t="s">
+      <c r="F4" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="49"/>
+      <c r="G4" s="51"/>
       <c r="H4" s="9"/>
       <c r="I4" s="7" t="s">
         <v>3</v>
@@ -1236,7 +1236,7 @@
       <c r="K4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="L4" s="57"/>
+      <c r="L4" s="46"/>
       <c r="N4" t="s">
         <v>5</v>
       </c>
@@ -1252,20 +1252,20 @@
         <f>A5*$N$5/100</f>
         <v>210</v>
       </c>
-      <c r="C5" s="52">
+      <c r="C5" s="54">
         <f>A5+B5</f>
         <v>1210</v>
       </c>
-      <c r="D5" s="53"/>
+      <c r="D5" s="55"/>
       <c r="E5" s="21">
         <f>C5*$O$5/100</f>
         <v>60.5</v>
       </c>
-      <c r="F5" s="50">
+      <c r="F5" s="52">
         <f>C5+E5</f>
         <v>1270.5</v>
       </c>
-      <c r="G5" s="51"/>
+      <c r="G5" s="53"/>
       <c r="H5" s="10"/>
       <c r="I5" s="27">
         <f>F5-(F5/(1+$N$5/100))</f>
@@ -1298,20 +1298,20 @@
         <f t="shared" ref="B6:B7" si="0">A6*$N$5/100</f>
         <v>420</v>
       </c>
-      <c r="C6" s="52">
+      <c r="C6" s="54">
         <f t="shared" ref="C6:C7" si="1">A6+B6</f>
         <v>2420</v>
       </c>
-      <c r="D6" s="53"/>
+      <c r="D6" s="55"/>
       <c r="E6" s="22">
         <f>C6*$O$5/100</f>
         <v>121</v>
       </c>
-      <c r="F6" s="52">
+      <c r="F6" s="54">
         <f>C6+E6</f>
         <v>2541</v>
       </c>
-      <c r="G6" s="53"/>
+      <c r="G6" s="55"/>
       <c r="H6" s="10"/>
       <c r="I6" s="28">
         <f>F6-(F6/(1+$N$5/100))</f>
@@ -1338,20 +1338,20 @@
         <f t="shared" si="0"/>
         <v>630</v>
       </c>
-      <c r="C7" s="54">
+      <c r="C7" s="56">
         <f t="shared" si="1"/>
         <v>3630</v>
       </c>
-      <c r="D7" s="55"/>
+      <c r="D7" s="57"/>
       <c r="E7" s="23">
         <f>C7*$O$5/100</f>
         <v>181.5</v>
       </c>
-      <c r="F7" s="54">
+      <c r="F7" s="56">
         <f>C7+E7</f>
         <v>3811.5</v>
       </c>
-      <c r="G7" s="55"/>
+      <c r="G7" s="57"/>
       <c r="H7" s="10"/>
       <c r="I7" s="29">
         <f>F7-(F7/(1+$N$5/100))</f>
@@ -1372,20 +1372,20 @@
     </row>
     <row r="8" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="46"/>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46"/>
-      <c r="J9" s="46"/>
-      <c r="K9" s="46"/>
-      <c r="L9" s="47"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="48"/>
+      <c r="L9" s="49"/>
     </row>
     <row r="10" spans="1:15" ht="6.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1403,7 +1403,7 @@
       </c>
       <c r="J11" s="43"/>
       <c r="K11" s="44"/>
-      <c r="L11" s="56" t="s">
+      <c r="L11" s="45" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1438,7 +1438,7 @@
       <c r="K12" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="L12" s="57"/>
+      <c r="L12" s="46"/>
     </row>
     <row r="13" spans="1:15" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="33">
@@ -1615,12 +1615,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A11:G11"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="A3:G3"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A9:L9"/>
     <mergeCell ref="F4:G4"/>
@@ -1631,6 +1625,12 @@
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A11:G11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="A3:G3"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>

</xml_diff>